<commit_message>
add new parameters checks
</commit_message>
<xml_diff>
--- a/params_v1.xlsx
+++ b/params_v1.xlsx
@@ -2,9 +2,9 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,14 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$E$77</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="81">
   <si>
     <t>func</t>
   </si>
@@ -231,10 +231,37 @@
     <t>Max</t>
   </si>
   <si>
-    <t>Any</t>
-  </si>
-  <si>
     <t>Required or Optional</t>
+  </si>
+  <si>
+    <t>func (multi params)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">, </t>
+  </si>
+  <si>
+    <t>));</t>
+  </si>
+  <si>
+    <t>MAX_LIMIT</t>
+  </si>
+  <si>
+    <t>functionsWithParams.add(new FunctionWithParameters(</t>
+  </si>
+  <si>
+    <t>unique formulas</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Conversion</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>IsBiggerThan()</t>
   </si>
 </sst>
 </file>
@@ -250,12 +277,42 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -350,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -362,6 +419,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,10 +733,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E69"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:N77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="B40" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38:L58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,45 +745,73 @@
     <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.28515625" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.7109375" customWidth="1"/>
+    <col min="12" max="12" width="61.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="G1" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="L1" s="18" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C2" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E2" s="15" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="G2" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>42</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>43</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -726,10 +825,30 @@
       <c r="E3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3" t="str">
+        <f>CONCATENATE("""",A3,"""")</f>
+        <v>"GetAncestry()"</v>
+      </c>
+      <c r="H3">
+        <f>D3</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f>E3</f>
+        <v>1</v>
+      </c>
+      <c r="J3" t="str">
+        <f>CONCATENATE("""",B3,"""")</f>
+        <v>"Boolean"</v>
+      </c>
+      <c r="L3" s="12" t="str">
+        <f>CONCATENATE($M$2,G3,$L$2,H3,$L$2,I3,$L$2,J3,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("GetAncestry()", 0, 1, "Boolean"));</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -743,13 +862,33 @@
       <c r="E4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G4" t="str">
+        <f t="shared" ref="G4:G35" si="0">CONCATENATE("""",A4,"""")</f>
+        <v>"GetDescendants()"</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H35" si="1">D4</f>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I35" si="2">E4</f>
+        <v>1</v>
+      </c>
+      <c r="J4" t="str">
+        <f>CONCATENATE("""",B4,"""")</f>
+        <v>"Boolean"</v>
+      </c>
+      <c r="L4" s="12" t="str">
+        <f>CONCATENATE($M$2,G4,$L$2,H4,$L$2,I4,$L$2,J4,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("GetDescendants()", 0, 1, "Boolean"));</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -760,10 +899,30 @@
       <c r="E5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>"ToLower()"</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J5" t="str">
+        <f>CONCATENATE("""",B5,"""")</f>
+        <v>"Boolean"</v>
+      </c>
+      <c r="L5" s="12" t="str">
+        <f>CONCATENATE($M$2,G5,$L$2,H5,$L$2,I5,$L$2,J5,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("ToLower()", 0, 1, "Boolean"));</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -777,27 +936,67 @@
       <c r="E6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>34</v>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>"ExtractDecimals()"</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J6" t="str">
+        <f>CONCATENATE("""",B6,"""")</f>
+        <v>"Double"</v>
+      </c>
+      <c r="L6" s="12" t="str">
+        <f>CONCATENATE($M$2,G6,$L$2,H6,$L$2,I6,$L$2,J6,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("ExtractDecimals()", 0, 1, "Double"));</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B7" t="s">
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>"GetDateTime()"</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J7" t="str">
+        <f>CONCATENATE("""",B7,"""")</f>
+        <v>"Double"</v>
+      </c>
+      <c r="L7" s="12" t="str">
+        <f>CONCATENATE($M$2,G7,$L$2,H7,$L$2,I7,$L$2,J7,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("GetDateTime()", 0, 1, "Double"));</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -811,10 +1010,30 @@
       <c r="E8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>"AtLeast()"</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J8" t="str">
+        <f>CONCATENATE("""",B8,"""")</f>
+        <v>"Double"</v>
+      </c>
+      <c r="L8" s="12" t="str">
+        <f>CONCATENATE($M$2,G8,$L$2,H8,$L$2,I8,$L$2,J8,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("AtLeast()", 1, 1, "Double"));</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
         <v>3</v>
@@ -828,44 +1047,104 @@
       <c r="E9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>"AtMost()"</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J9" t="str">
+        <f>CONCATENATE("""",B9,"""")</f>
+        <v>"Double"</v>
+      </c>
+      <c r="L9" s="12" t="str">
+        <f>CONCATENATE($M$2,G9,$L$2,H9,$L$2,I9,$L$2,J9,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("AtMost()", 1, 1, "Double"));</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>"MultiplyBy()"</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J10" t="str">
+        <f>CONCATENATE("""",B10,"""")</f>
+        <v>"Double"</v>
+      </c>
+      <c r="L10" s="12" t="str">
+        <f>CONCATENATE($M$2,G10,$L$2,H10,$L$2,I10,$L$2,J10,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("MultiplyBy()", 1, 1, "Double"));</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>30</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>50</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>"ToTitleCase()"</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J11" t="str">
+        <f>CONCATENATE("""",B11,"""")</f>
+        <v>"Int32"</v>
+      </c>
+      <c r="L11" s="12" t="str">
+        <f>CONCATENATE($M$2,G11,$L$2,H11,$L$2,I11,$L$2,J11,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("ToTitleCase()", 0, 1, "Int32"));</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
@@ -879,10 +1158,30 @@
       <c r="E12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>"GetLine()"</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J12" t="str">
+        <f>CONCATENATE("""",B12,"""")</f>
+        <v>"Int32"</v>
+      </c>
+      <c r="L12" s="12" t="str">
+        <f>CONCATENATE($M$2,G12,$L$2,H12,$L$2,I12,$L$2,J12,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("GetLine()", 1, 1, "Int32"));</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
@@ -896,10 +1195,30 @@
       <c r="E13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>"GetLineBody()"</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J13" t="str">
+        <f>CONCATENATE("""",B13,"""")</f>
+        <v>"Int32"</v>
+      </c>
+      <c r="L13" s="12" t="str">
+        <f>CONCATENATE($M$2,G13,$L$2,H13,$L$2,I13,$L$2,J13,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("GetLineBody()", 1, 1, "Int32"));</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
@@ -913,27 +1232,67 @@
       <c r="E14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G14" t="str">
+        <f t="shared" si="0"/>
+        <v>"Skip()"</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J14" t="str">
+        <f>CONCATENATE("""",B14,"""")</f>
+        <v>"Int32"</v>
+      </c>
+      <c r="L14" s="12" t="str">
+        <f>CONCATENATE($M$2,G14,$L$2,H14,$L$2,I14,$L$2,J14,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("Skip()", 1, 1, "Int32"));</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>"Take()"</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J15" t="str">
+        <f>CONCATENATE("""",B15,"""")</f>
+        <v>"Int32"</v>
+      </c>
+      <c r="L15" s="12" t="str">
+        <f>CONCATENATE($M$2,G15,$L$2,H15,$L$2,I15,$L$2,J15,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("Take()", 1, 1, "Int32"));</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>5</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
@@ -947,10 +1306,30 @@
       <c r="E16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G16" t="str">
+        <f t="shared" si="0"/>
+        <v>"Flatten()"</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J16" t="str">
+        <f>CONCATENATE("""",B16,"""")</f>
+        <v>"String"</v>
+      </c>
+      <c r="L16" s="12" t="str">
+        <f>CONCATENATE($M$2,G16,$L$2,H16,$L$2,I16,$L$2,J16,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("Flatten()", 0, 1, "String"));</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="B17" t="s">
         <v>6</v>
@@ -964,27 +1343,67 @@
       <c r="E17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G17" t="str">
+        <f t="shared" si="0"/>
+        <v>"GetFullColorDescription()"</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J17" t="str">
+        <f>CONCATENATE("""",B17,"""")</f>
+        <v>"String"</v>
+      </c>
+      <c r="L17" s="12" t="str">
+        <f>CONCATENATE($M$2,G17,$L$2,H17,$L$2,I17,$L$2,J17,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("GetFullColorDescription()", 0, 1, "String"));</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="B18" t="s">
         <v>6</v>
       </c>
       <c r="C18" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G18" t="str">
+        <f t="shared" si="0"/>
+        <v>"ListPaths()"</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J18" t="str">
+        <f>CONCATENATE("""",B18,"""")</f>
+        <v>"String"</v>
+      </c>
+      <c r="L18" s="12" t="str">
+        <f>CONCATENATE($M$2,G18,$L$2,H18,$L$2,I18,$L$2,J18,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("ListPaths()", 0, 1, "String"));</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
         <v>6</v>
@@ -998,10 +1417,30 @@
       <c r="E19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G19" t="str">
+        <f t="shared" si="0"/>
+        <v>"EraseTextSurroundedBy()"</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J19" t="str">
+        <f>CONCATENATE("""",B19,"""")</f>
+        <v>"String"</v>
+      </c>
+      <c r="L19" s="12" t="str">
+        <f>CONCATENATE($M$2,G19,$L$2,H19,$L$2,I19,$L$2,J19,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("EraseTextSurroundedBy()", 1, 1, "String"));</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>44</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
@@ -1015,10 +1454,30 @@
       <c r="E20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G20" t="str">
+        <f t="shared" si="0"/>
+        <v>"Format()"</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J20" t="str">
+        <f>CONCATENATE("""",B20,"""")</f>
+        <v>"String"</v>
+      </c>
+      <c r="L20" s="12" t="str">
+        <f>CONCATENATE($M$2,G20,$L$2,H20,$L$2,I20,$L$2,J20,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("Format()", 1, 1, "String"));</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
@@ -1032,10 +1491,30 @@
       <c r="E21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G21" t="str">
+        <f t="shared" si="0"/>
+        <v>"IsDescendantOf()"</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J21" t="str">
+        <f>CONCATENATE("""",B21,"""")</f>
+        <v>"String"</v>
+      </c>
+      <c r="L21" s="12" t="str">
+        <f>CONCATENATE($M$2,G21,$L$2,H21,$L$2,I21,$L$2,J21,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("IsDescendantOf()", 1, 1, "String"));</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
         <v>6</v>
@@ -1049,10 +1528,30 @@
       <c r="E22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G22" t="str">
+        <f t="shared" si="0"/>
+        <v>"Postfix()"</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J22" t="str">
+        <f>CONCATENATE("""",B22,"""")</f>
+        <v>"String"</v>
+      </c>
+      <c r="L22" s="12" t="str">
+        <f>CONCATENATE($M$2,G22,$L$2,H22,$L$2,I22,$L$2,J22,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("Postfix()", 1, 1, "String"));</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
@@ -1066,44 +1565,104 @@
       <c r="E23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G23" t="str">
+        <f t="shared" si="0"/>
+        <v>"Prefix()"</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J23" t="str">
+        <f>CONCATENATE("""",B23,"""")</f>
+        <v>"String"</v>
+      </c>
+      <c r="L23" s="12" t="str">
+        <f>CONCATENATE($M$2,G23,$L$2,H23,$L$2,I23,$L$2,J23,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("Prefix()", 1, 1, "String"));</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="0"/>
+        <v>"ToText()"</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J24" t="str">
+        <f>CONCATENATE("""",B24,"""")</f>
+        <v>"String"</v>
+      </c>
+      <c r="L24" s="12" t="str">
+        <f>CONCATENATE($M$2,G24,$L$2,H24,$L$2,I24,$L$2,J24,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("ToText()", 1, 1, "String"));</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>38</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>39</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>7</v>
       </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>74</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="0"/>
+        <v>"Match()"</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I25" t="str">
+        <f t="shared" si="2"/>
+        <v>MAX_LIMIT</v>
+      </c>
+      <c r="J25" t="str">
+        <f>CONCATENATE("""",B25,"""")</f>
+        <v>"Int32[]"</v>
+      </c>
+      <c r="L25" s="12" t="str">
+        <f>CONCATENATE($M$2,G25,$L$2,H25,$L$2,I25,$L$2,J25,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("Match()", 0, MAX_LIMIT, "Int32[]"));</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>25</v>
-      </c>
-      <c r="B25" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>31</v>
       </c>
       <c r="B26" t="s">
         <v>26</v>
@@ -1115,12 +1674,32 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="0"/>
+        <v>"Split()"</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I26" t="str">
+        <f t="shared" si="2"/>
+        <v>MAX_LIMIT</v>
+      </c>
+      <c r="J26" t="str">
+        <f>CONCATENATE("""",B26,"""")</f>
+        <v>"String[]"</v>
+      </c>
+      <c r="L26" s="12" t="str">
+        <f>CONCATENATE($M$2,G26,$L$2,H26,$L$2,I26,$L$2,J26,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("Split()", 1, MAX_LIMIT, "String[]"));</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
         <v>26</v>
@@ -1132,12 +1711,32 @@
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="0"/>
+        <v>"UseSeparators()"</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I27" t="str">
+        <f t="shared" si="2"/>
+        <v>MAX_LIMIT</v>
+      </c>
+      <c r="J27" t="str">
+        <f>CONCATENATE("""",B27,"""")</f>
+        <v>"String[]"</v>
+      </c>
+      <c r="L27" s="12" t="str">
+        <f>CONCATENATE($M$2,G27,$L$2,H27,$L$2,I27,$L$2,J27,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("UseSeparators()", 1, MAX_LIMIT, "String[]"));</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
         <v>26</v>
@@ -1149,12 +1748,32 @@
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="0"/>
+        <v>"Where()"</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I28" t="str">
+        <f t="shared" si="2"/>
+        <v>MAX_LIMIT</v>
+      </c>
+      <c r="J28" t="str">
+        <f>CONCATENATE("""",B28,"""")</f>
+        <v>"String[]"</v>
+      </c>
+      <c r="L28" s="12" t="str">
+        <f>CONCATENATE($M$2,G28,$L$2,H28,$L$2,I28,$L$2,J28,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("Where()", 1, MAX_LIMIT, "String[]"));</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B29" t="s">
         <v>26</v>
@@ -1166,12 +1785,32 @@
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="0"/>
+        <v>"WhereNot()"</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I29" t="str">
+        <f t="shared" si="2"/>
+        <v>MAX_LIMIT</v>
+      </c>
+      <c r="J29" t="str">
+        <f>CONCATENATE("""",B29,"""")</f>
+        <v>"String[]"</v>
+      </c>
+      <c r="L29" s="12" t="str">
+        <f>CONCATENATE($M$2,G29,$L$2,H29,$L$2,I29,$L$2,J29,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("WhereNot()", 1, MAX_LIMIT, "String[]"));</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
         <v>26</v>
@@ -1183,12 +1822,32 @@
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="0"/>
+        <v>"WhereUnit()"</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I30" t="str">
+        <f t="shared" si="2"/>
+        <v>MAX_LIMIT</v>
+      </c>
+      <c r="J30" t="str">
+        <f>CONCATENATE("""",B30,"""")</f>
+        <v>"String[]"</v>
+      </c>
+      <c r="L30" s="12" t="str">
+        <f>CONCATENATE($M$2,G30,$L$2,H30,$L$2,I30,$L$2,J30,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("WhereUnit()", 1, MAX_LIMIT, "String[]"));</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
         <v>26</v>
@@ -1200,12 +1859,32 @@
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="0"/>
+        <v>"WhereUnitOrValue()"</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I31" t="str">
+        <f t="shared" si="2"/>
+        <v>MAX_LIMIT</v>
+      </c>
+      <c r="J31" t="str">
+        <f>CONCATENATE("""",B31,"""")</f>
+        <v>"String[]"</v>
+      </c>
+      <c r="L31" s="12" t="str">
+        <f>CONCATENATE($M$2,G31,$L$2,H31,$L$2,I31,$L$2,J31,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("WhereUnitOrValue()", 1, MAX_LIMIT, "String[]"));</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" t="s">
         <v>26</v>
@@ -1217,12 +1896,32 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="0"/>
+        <v>"WhereCategory()"</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I32" t="str">
+        <f t="shared" si="2"/>
+        <v>MAX_LIMIT</v>
+      </c>
+      <c r="J32" t="str">
+        <f>CONCATENATE("""",B32,"""")</f>
+        <v>"String[]"</v>
+      </c>
+      <c r="L32" s="12" t="str">
+        <f>CONCATENATE($M$2,G32,$L$2,H32,$L$2,I32,$L$2,J32,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("WhereCategory()", 1, MAX_LIMIT, "String[]"));</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
         <v>26</v>
@@ -1234,12 +1933,32 @@
         <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v>"WhereManufacturer()"</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I33" t="str">
+        <f t="shared" si="2"/>
+        <v>MAX_LIMIT</v>
+      </c>
+      <c r="J33" t="str">
+        <f>CONCATENATE("""",B33,"""")</f>
+        <v>"String[]"</v>
+      </c>
+      <c r="L33" s="12" t="str">
+        <f>CONCATENATE($M$2,G33,$L$2,H33,$L$2,I33,$L$2,J33,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("WhereManufacturer()", 1, MAX_LIMIT, "String[]"));</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B34" t="s">
         <v>26</v>
@@ -1251,122 +1970,265 @@
         <v>1</v>
       </c>
       <c r="E34" t="s">
+        <v>74</v>
+      </c>
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v>"WhereModelName()"</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I34" t="str">
+        <f t="shared" si="2"/>
+        <v>MAX_LIMIT</v>
+      </c>
+      <c r="J34" t="str">
+        <f>CONCATENATE("""",B34,"""")</f>
+        <v>"String[]"</v>
+      </c>
+      <c r="L34" s="12" t="str">
+        <f>CONCATENATE($M$2,G34,$L$2,H34,$L$2,I34,$L$2,J34,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("WhereModelName()", 1, MAX_LIMIT, "String[]"));</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>74</v>
+      </c>
+      <c r="G35" t="str">
+        <f t="shared" si="0"/>
+        <v>"WhereProductLine()"</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I35" t="str">
+        <f t="shared" si="2"/>
+        <v>MAX_LIMIT</v>
+      </c>
+      <c r="J35" t="str">
+        <f>CONCATENATE("""",B35,"""")</f>
+        <v>"String[]"</v>
+      </c>
+      <c r="L35" s="12" t="str">
+        <f>CONCATENATE($M$2,G35,$L$2,H35,$L$2,I35,$L$2,J35,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("WhereProductLine()", 1, MAX_LIMIT, "String[]"));</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="15" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="D37" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G37" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="I37" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="J37" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K37" s="12"/>
+      <c r="L37" s="16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" s="3">
+      <c r="C38" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="3">
         <v>2</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E38" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-      <c r="B36" s="9" t="s">
+      <c r="G38" t="str">
+        <f t="shared" ref="G38:G57" si="3">CONCATENATE("""",A38,"""")</f>
+        <v>"IfLike()"</v>
+      </c>
+      <c r="H38">
+        <f t="shared" ref="H38:H57" si="4">D38</f>
+        <v>2</v>
+      </c>
+      <c r="I38">
+        <f t="shared" ref="I38:I57" si="5">E38</f>
+        <v>2</v>
+      </c>
+      <c r="J38" t="str">
+        <f>CONCATENATE("""",B38,"""")</f>
+        <v>"String"</v>
+      </c>
+      <c r="L38" s="13" t="str">
+        <f>CONCATENATE($M$2,G38,$L$2,H38,$L$2,I38,$L$2,J38,$L$2,J39,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("IfLike()", 2, 2, "String", "String"));</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="8"/>
+      <c r="B39" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" s="9"/>
-      <c r="E36" s="10"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="C39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="9"/>
+      <c r="E39" s="10"/>
+      <c r="G39" t="str">
+        <f t="shared" si="3"/>
+        <v>""</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J39" t="str">
+        <f>CONCATENATE("""",B39,"""")</f>
+        <v>"String"</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B40" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37" s="3">
+      <c r="C40" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="3">
         <v>2</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E40" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="9" t="s">
+      <c r="G40" t="str">
+        <f t="shared" si="3"/>
+        <v>"IfLongerThan()"</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="J40" t="str">
+        <f>CONCATENATE("""",B40,"""")</f>
+        <v>"Int32"</v>
+      </c>
+      <c r="L40" s="13" t="str">
+        <f>CONCATENATE($M$2,G40,$L$2,H40,$L$2,I40,$L$2,J40,$L$2,J41,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("IfLongerThan()", 2, 2, "Int32", "String"));</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="B41" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" s="9"/>
-      <c r="E38" s="10"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="C41" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="9"/>
+      <c r="E41" s="10"/>
+      <c r="G41" t="str">
+        <f t="shared" si="3"/>
+        <v>""</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J41" t="str">
+        <f>CONCATENATE("""",B41,"""")</f>
+        <v>"String"</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B42" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C42" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D39" s="3">
-        <v>0</v>
-      </c>
-      <c r="E39" s="4">
+      <c r="D42" s="3">
+        <v>0</v>
+      </c>
+      <c r="E42" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C40" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D40" s="9"/>
-      <c r="E40" s="10"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" s="3">
-        <v>1</v>
-      </c>
-      <c r="E41" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C42" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D42" s="6"/>
-      <c r="E42" s="7"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G42" t="str">
+        <f t="shared" si="3"/>
+        <v>"FlattenWithAnd()"</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="J42" t="str">
+        <f>CONCATENATE("""",B42,"""")</f>
+        <v>"Int32"</v>
+      </c>
+      <c r="L42" s="13" t="str">
+        <f>CONCATENATE($M$2,G42,$L$2,H42,$L$2,I42,$L$2,J42,$L$2,J43,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("FlattenWithAnd()", 0, 2, "Int32", "String"));</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="8"/>
       <c r="B43" s="9" t="s">
         <v>6</v>
@@ -1376,8 +2238,24 @@
       </c>
       <c r="D43" s="9"/>
       <c r="E43" s="10"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G43" t="str">
+        <f t="shared" si="3"/>
+        <v>""</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J43" t="str">
+        <f>CONCATENATE("""",B43,"""")</f>
+        <v>"String"</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>21</v>
       </c>
@@ -1393,8 +2271,28 @@
       <c r="E44" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G44" t="str">
+        <f t="shared" si="3"/>
+        <v>"RegexReplace()"</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="J44" t="str">
+        <f>CONCATENATE("""",B44,"""")</f>
+        <v>"String"</v>
+      </c>
+      <c r="L44" s="13" t="str">
+        <f>CONCATENATE($M$2,G44,$L$2,H44,$L$2,I44,$L$2,J44,$L$2,J45,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("RegexReplace()", 2, 2, "String", "String"));</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="9" t="s">
         <v>6</v>
@@ -1404,239 +2302,508 @@
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="10"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G45" t="str">
+        <f t="shared" si="3"/>
+        <v>""</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J45" t="str">
+        <f>CONCATENATE("""",B45,"""")</f>
+        <v>"String"</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D46" s="3">
+        <v>0</v>
+      </c>
+      <c r="E46" s="4">
         <v>2</v>
       </c>
-      <c r="E46" s="4">
+      <c r="G46" t="str">
+        <f>CONCATENATE("""",A46,"""")</f>
+        <v>"ListUSM()"</v>
+      </c>
+      <c r="H46">
+        <f>D46</f>
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <f>E46</f>
+        <v>2</v>
+      </c>
+      <c r="J46" t="str">
+        <f>CONCATENATE("""",B46,"""")</f>
+        <v>"String"</v>
+      </c>
+      <c r="L46" s="13" t="str">
+        <f>CONCATENATE($M$2,G46,$L$2,H46,$L$2,I46,$L$2,J46,$L$2,J47,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("ListUSM()", 0, 2, "String", "String"));</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" s="8"/>
+      <c r="B47" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="9"/>
+      <c r="E47" s="10"/>
+      <c r="G47" t="str">
+        <f>CONCATENATE("""",A47,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="H47">
+        <f>D47</f>
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <f>E47</f>
+        <v>0</v>
+      </c>
+      <c r="J47" t="str">
+        <f>CONCATENATE("""",B47,"""")</f>
+        <v>"String"</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="3">
+        <v>1</v>
+      </c>
+      <c r="E48" s="4">
+        <v>3</v>
+      </c>
+      <c r="G48" t="str">
+        <f>CONCATENATE("""",A48,"""")</f>
+        <v>"Erase()"</v>
+      </c>
+      <c r="H48">
+        <f>D48</f>
+        <v>1</v>
+      </c>
+      <c r="I48">
+        <f>E48</f>
+        <v>3</v>
+      </c>
+      <c r="J48" t="str">
+        <f>CONCATENATE("""",B48,"""")</f>
+        <v>"String"</v>
+      </c>
+      <c r="L48" s="13" t="str">
+        <f>CONCATENATE($M$2,G48,$L$2,H48,$L$2,I48,$L$2,J48,$L$2,J49,$L$2,J50,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("Erase()", 1, 3, "String", "Boolean", "String"));</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" s="6"/>
+      <c r="E49" s="7"/>
+      <c r="G49" t="str">
+        <f>CONCATENATE("""",A49,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="H49">
+        <f>D49</f>
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <f>E49</f>
+        <v>0</v>
+      </c>
+      <c r="J49" t="str">
+        <f>CONCATENATE("""",B49,"""")</f>
+        <v>"Boolean"</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" s="8"/>
+      <c r="B50" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" s="9"/>
+      <c r="E50" s="10"/>
+      <c r="G50" t="str">
+        <f>CONCATENATE("""",A50,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="H50">
+        <f>D50</f>
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <f>E50</f>
+        <v>0</v>
+      </c>
+      <c r="J50" t="str">
+        <f>CONCATENATE("""",B50,"""")</f>
+        <v>"String"</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" s="3">
+        <v>1</v>
+      </c>
+      <c r="E51" s="4">
+        <v>3</v>
+      </c>
+      <c r="G51" t="str">
+        <f>CONCATENATE("""",A51,"""")</f>
+        <v>"Shorten()"</v>
+      </c>
+      <c r="H51">
+        <f>D51</f>
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <f>E51</f>
+        <v>3</v>
+      </c>
+      <c r="J51" t="str">
+        <f>CONCATENATE("""",B51,"""")</f>
+        <v>"Int32"</v>
+      </c>
+      <c r="L51" s="13" t="str">
+        <f>CONCATENATE($M$2,G51,$L$2,H51,$L$2,I51,$L$2,J51,$L$2,J52,$L$2,J53,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("Shorten()", 1, 3, "Int32", "String", "String"));</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="5"/>
+      <c r="B52" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="6"/>
+      <c r="E52" s="7"/>
+      <c r="G52" t="str">
+        <f>CONCATENATE("""",A52,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="H52">
+        <f>D52</f>
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <f>E52</f>
+        <v>0</v>
+      </c>
+      <c r="J52" t="str">
+        <f>CONCATENATE("""",B52,"""")</f>
+        <v>"String"</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="8"/>
+      <c r="B53" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="9"/>
+      <c r="E53" s="10"/>
+      <c r="G53" t="str">
+        <f>CONCATENATE("""",A53,"""")</f>
+        <v>""</v>
+      </c>
+      <c r="H53">
+        <f>D53</f>
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <f>E53</f>
+        <v>0</v>
+      </c>
+      <c r="J53" t="str">
+        <f>CONCATENATE("""",B53,"""")</f>
+        <v>"String"</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="3">
+        <v>2</v>
+      </c>
+      <c r="E54" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="6" t="s">
+      <c r="G54" t="str">
+        <f t="shared" si="3"/>
+        <v>"Replace()"</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="J54" t="str">
+        <f>CONCATENATE("""",B54,"""")</f>
+        <v>"String"</v>
+      </c>
+      <c r="L54" s="13" t="str">
+        <f>CONCATENATE($M$2,G54,$L$2,H54,$L$2,I54,$L$2,J54,$L$2,J55,$L$2,J56,$L$2,J57,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("Replace()", 2, 4, "String", "String", "String", "StringComparison"));</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="5"/>
+      <c r="B55" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D47" s="6"/>
-      <c r="E47" s="7"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="5"/>
-      <c r="B48" s="6" t="s">
+      <c r="C55" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="6"/>
+      <c r="E55" s="7"/>
+      <c r="G55" t="str">
+        <f t="shared" si="3"/>
+        <v>""</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J55" t="str">
+        <f>CONCATENATE("""",B55,"""")</f>
+        <v>"String"</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="5"/>
+      <c r="B56" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C56" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D48" s="6"/>
-      <c r="E48" s="7"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="8"/>
-      <c r="B49" s="9" t="s">
+      <c r="D56" s="6"/>
+      <c r="E56" s="7"/>
+      <c r="G56" t="str">
+        <f t="shared" si="3"/>
+        <v>""</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J56" t="str">
+        <f>CONCATENATE("""",B56,"""")</f>
+        <v>"String"</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="8"/>
+      <c r="B57" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C49" s="9" t="s">
+      <c r="C57" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D49" s="9"/>
-      <c r="E49" s="10"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D50" s="3">
-        <v>1</v>
-      </c>
-      <c r="E50" s="4">
+      <c r="D57" s="9"/>
+      <c r="E57" s="10"/>
+      <c r="G57" t="str">
+        <f t="shared" si="3"/>
+        <v>""</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J57" t="str">
+        <f>CONCATENATE("""",B57,"""")</f>
+        <v>"StringComparison"</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B58" s="20" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
-      <c r="B51" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D51" s="6"/>
-      <c r="E51" s="7"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="8"/>
-      <c r="B52" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D52" s="9"/>
-      <c r="E52" s="10"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D53" s="3">
-        <v>0</v>
-      </c>
-      <c r="E53" s="4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="8"/>
-      <c r="B54" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D54" s="9"/>
-      <c r="E54" s="10"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="C58" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" s="3">
+        <v>4</v>
+      </c>
+      <c r="E58" s="4">
+        <v>4</v>
+      </c>
+      <c r="G58" t="str">
+        <f t="shared" ref="G58:G61" si="6">CONCATENATE("""",A58,"""")</f>
+        <v>"IsBiggerThan()"</v>
+      </c>
+      <c r="H58">
+        <f t="shared" ref="H58:H61" si="7">D58</f>
+        <v>4</v>
+      </c>
+      <c r="I58">
+        <f t="shared" ref="I58:I61" si="8">E58</f>
+        <v>4</v>
+      </c>
+      <c r="J58" t="str">
+        <f t="shared" ref="J58:J61" si="9">CONCATENATE("""",B58,"""")</f>
+        <v>"Double"</v>
+      </c>
+      <c r="L58" s="13" t="str">
+        <f>CONCATENATE($M$2,G58,$L$2,H58,$L$2,I58,$L$2,J58,$L$2,J59,$L$2,J60,$L$2,J61,$N$2)</f>
+        <v>functionsWithParams.add(new FunctionWithParameters("IsBiggerThan()", 4, 4, "Double", "Double", "Double", "Double"));</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="5"/>
+      <c r="B59" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" s="6"/>
+      <c r="E59" s="7"/>
+      <c r="G59" t="str">
+        <f t="shared" si="6"/>
+        <v>""</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J59" t="str">
+        <f t="shared" si="9"/>
+        <v>"Double"</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="5"/>
+      <c r="B60" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60" s="6"/>
+      <c r="E60" s="7"/>
+      <c r="G60" t="str">
+        <f t="shared" si="6"/>
+        <v>""</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J60" t="str">
+        <f t="shared" si="9"/>
+        <v>"Double"</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="8"/>
+      <c r="B61" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" s="9"/>
+      <c r="E61" s="10"/>
+      <c r="G61" t="str">
+        <f t="shared" si="6"/>
+        <v>""</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J61" t="str">
+        <f t="shared" si="9"/>
+        <v>"Double"</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>52</v>
-      </c>
-      <c r="B55" t="s">
-        <v>53</v>
-      </c>
-      <c r="D55">
-        <v>0</v>
-      </c>
-      <c r="E55">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B56" t="s">
-        <v>53</v>
-      </c>
-      <c r="D56">
-        <v>0</v>
-      </c>
-      <c r="E56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>55</v>
-      </c>
-      <c r="B57" t="s">
-        <v>53</v>
-      </c>
-      <c r="D57">
-        <v>0</v>
-      </c>
-      <c r="E57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>56</v>
-      </c>
-      <c r="B58" t="s">
-        <v>53</v>
-      </c>
-      <c r="D58">
-        <v>0</v>
-      </c>
-      <c r="E58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>57</v>
-      </c>
-      <c r="B59" t="s">
-        <v>53</v>
-      </c>
-      <c r="D59">
-        <v>0</v>
-      </c>
-      <c r="E59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>58</v>
-      </c>
-      <c r="B60" t="s">
-        <v>53</v>
-      </c>
-      <c r="D60">
-        <v>0</v>
-      </c>
-      <c r="E60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>59</v>
-      </c>
-      <c r="B61" t="s">
-        <v>53</v>
-      </c>
-      <c r="D61">
-        <v>0</v>
-      </c>
-      <c r="E61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>60</v>
-      </c>
-      <c r="B62" t="s">
-        <v>53</v>
-      </c>
-      <c r="D62">
-        <v>0</v>
-      </c>
-      <c r="E62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>61</v>
       </c>
       <c r="B63" t="s">
         <v>53</v>
@@ -1648,9 +2815,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B64" t="s">
         <v>53</v>
@@ -1664,7 +2831,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B65" t="s">
         <v>53</v>
@@ -1678,7 +2845,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B66" t="s">
         <v>53</v>
@@ -1692,7 +2859,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B67" t="s">
         <v>53</v>
@@ -1706,7 +2873,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B68" t="s">
         <v>53</v>
@@ -1720,7 +2887,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="B69" t="s">
         <v>53</v>
@@ -1732,19 +2899,136 @@
         <v>0</v>
       </c>
     </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>60</v>
+      </c>
+      <c r="B70" t="s">
+        <v>53</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>61</v>
+      </c>
+      <c r="B71" t="s">
+        <v>53</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>62</v>
+      </c>
+      <c r="B72" t="s">
+        <v>53</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>63</v>
+      </c>
+      <c r="B73" t="s">
+        <v>53</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>64</v>
+      </c>
+      <c r="B74" t="s">
+        <v>53</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>65</v>
+      </c>
+      <c r="B75" t="s">
+        <v>53</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>66</v>
+      </c>
+      <c r="B76" t="s">
+        <v>53</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>67</v>
+      </c>
+      <c r="B77" t="s">
+        <v>53</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E49"/>
+  <autoFilter ref="A2:E57"/>
   <sortState ref="A2:E23">
     <sortCondition ref="B2:B23"/>
     <sortCondition ref="C2:C23"/>
     <sortCondition ref="A2:A23"/>
   </sortState>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:J1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1757,6 +3041,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
fixed issue with empty parameters in the Split function
</commit_message>
<xml_diff>
--- a/params_v1.xlsx
+++ b/params_v1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$E$78</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -739,8 +739,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView tabSelected="1" topLeftCell="G13" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1711,7 +1711,7 @@
         <v>9</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" t="s">
         <v>74</v>
@@ -1722,7 +1722,7 @@
       </c>
       <c r="H27">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I27" t="str">
         <f t="shared" si="4"/>
@@ -1734,7 +1734,7 @@
       </c>
       <c r="L27" s="12" t="str">
         <f t="shared" si="1"/>
-        <v>functionsWithParams.add(new FunctionWithParameters("Split()", 1, MAX_LIMIT, "String[]"));</v>
+        <v>functionsWithParams.add(new FunctionWithParameters("Split()", 0, MAX_LIMIT, "String[]"));</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix empty parameters of UseSeparator's function
</commit_message>
<xml_diff>
--- a/params_v1.xlsx
+++ b/params_v1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$E$78</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -739,8 +739,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:N78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G13" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1758,8 +1758,7 @@
         <v>"UseSeparators()"</v>
       </c>
       <c r="H28">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I28" t="str">
         <f t="shared" si="4"/>
@@ -1771,7 +1770,7 @@
       </c>
       <c r="L28" s="12" t="str">
         <f t="shared" si="1"/>
-        <v>functionsWithParams.add(new FunctionWithParameters("UseSeparators()", 1, MAX_LIMIT, "String[]"));</v>
+        <v>functionsWithParams.add(new FunctionWithParameters("UseSeparators()", 0, MAX_LIMIT, "String[]"));</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>